<commit_message>
data collected and recorded in the protocol
</commit_message>
<xml_diff>
--- a/result_tests.xlsx
+++ b/result_tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\permi\source\repos\university\os\2_merge_sort\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\permi\source\repos\university\os\3_merge_sort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ED16C98-79D0-4931-9567-643F9300738F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318B4D38-7D58-4C40-BAD1-502BA97F26CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11505" xr2:uid="{66067D0F-0414-489E-B181-C182FD2DCA62}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{66067D0F-0414-489E-B181-C182FD2DCA62}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>tests</t>
   </si>
@@ -51,34 +51,43 @@
     <t>count elements</t>
   </si>
   <si>
-    <t>3.697</t>
-  </si>
-  <si>
-    <t>400.045</t>
-  </si>
-  <si>
-    <t>3.835</t>
-  </si>
-  <si>
-    <t>5.945</t>
-  </si>
-  <si>
-    <t>3.032</t>
-  </si>
-  <si>
-    <t>3.102</t>
-  </si>
-  <si>
-    <t>452.451</t>
-  </si>
-  <si>
-    <t>405.115</t>
-  </si>
-  <si>
-    <t>424.439</t>
-  </si>
-  <si>
-    <t>404.212</t>
+    <t>single thread</t>
+  </si>
+  <si>
+    <t>0.332334</t>
+  </si>
+  <si>
+    <t>0.207382</t>
+  </si>
+  <si>
+    <t>0.100345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.185292 </t>
+  </si>
+  <si>
+    <t>0.090462</t>
+  </si>
+  <si>
+    <t>0.107350</t>
+  </si>
+  <si>
+    <t>0.000648</t>
+  </si>
+  <si>
+    <t>0.000714</t>
+  </si>
+  <si>
+    <t>0.000832</t>
+  </si>
+  <si>
+    <t>0.000205</t>
+  </si>
+  <si>
+    <t>0.002012</t>
+  </si>
+  <si>
+    <t>0.003812</t>
   </si>
 </sst>
 </file>
@@ -431,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1411F7-89A0-42FC-A2D7-BC4B5630C7E0}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +464,7 @@
         <v>1000</v>
       </c>
       <c r="C2">
-        <v>100000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,10 +472,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -474,10 +483,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -485,10 +494,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -496,10 +505,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -507,13 +516,25 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>